<commit_message>
Clean up DESeq analysis
- better summary
- updated for current version of R
- ggVennDiagram uses geom_polygon and geom_text, not geom_sf
</commit_message>
<xml_diff>
--- a/input_experiment/Gat201_samplesheet.xlsx
+++ b/input_experiment/Gat201_samplesheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth\Documents\GitHub\CryptoGat201RNASeq_draft\input_experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ewallac2/Repos/CryptoGat201RNASeq/input_experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D9ADB3-8992-1A4E-B4F8-C7633845DD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9375"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="24000" windowHeight="9380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gat201_samplesheet" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="47">
   <si>
     <t>SampleID</t>
   </si>
@@ -28,9 +29,6 @@
   </si>
   <si>
     <t>Media</t>
-  </si>
-  <si>
-    <t>Timepoint</t>
   </si>
   <si>
     <t>Group</t>
@@ -168,7 +166,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -968,14 +966,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -997,22 +997,19 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -1020,14 +1017,11 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2">
+      <c r="G2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1035,25 +1029,22 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1061,25 +1052,22 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
         <v>120</v>
       </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1087,36 +1075,33 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5">
         <v>240</v>
       </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>8</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -1124,14 +1109,11 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6">
+      <c r="G6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1139,25 +1121,22 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="D7">
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1165,25 +1144,22 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
         <v>120</v>
       </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1191,25 +1167,22 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
         <v>240</v>
       </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1217,25 +1190,22 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="D10">
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10">
         <v>30</v>
       </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1243,51 +1213,45 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11">
         <v>120</v>
       </c>
-      <c r="E11" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="F11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12">
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12">
         <v>240</v>
       </c>
-      <c r="E12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1295,51 +1259,45 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
         <v>18</v>
       </c>
-      <c r="D13">
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13">
         <v>30</v>
       </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
         <v>20</v>
       </c>
-      <c r="H13">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14">
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14">
         <v>120</v>
       </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1347,25 +1305,22 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15">
         <v>240</v>
       </c>
-      <c r="E15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1373,25 +1328,22 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
       </c>
       <c r="E16" t="s">
         <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="G16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1399,51 +1351,45 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17">
         <v>30</v>
       </c>
-      <c r="E17" t="s">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
         <v>25</v>
       </c>
-      <c r="F17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18">
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18">
         <v>120</v>
       </c>
-      <c r="E18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1451,25 +1397,22 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19">
         <v>240</v>
       </c>
-      <c r="E19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1477,25 +1420,22 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
       </c>
       <c r="E20" t="s">
         <v>23</v>
       </c>
       <c r="F20" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="G20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1503,25 +1443,22 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21">
         <v>30</v>
       </c>
-      <c r="E21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1529,25 +1466,22 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22">
         <v>120</v>
       </c>
-      <c r="E22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1555,25 +1489,22 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23">
         <v>240</v>
       </c>
-      <c r="E23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1581,25 +1512,22 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24">
         <v>30</v>
       </c>
-      <c r="E24" t="s">
-        <v>28</v>
-      </c>
-      <c r="F24" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1607,25 +1535,22 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25">
         <v>120</v>
       </c>
-      <c r="E25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1633,25 +1558,22 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26">
         <v>240</v>
       </c>
-      <c r="E26" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1659,25 +1581,22 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27">
         <v>30</v>
       </c>
-      <c r="E27" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1685,25 +1604,22 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28">
+        <v>17</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28">
         <v>120</v>
       </c>
-      <c r="E28" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1711,51 +1627,45 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29">
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29">
         <v>240</v>
       </c>
-      <c r="E29" t="s">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>30</v>
       </c>
-      <c r="F29" t="s">
-        <v>24</v>
-      </c>
-      <c r="G29" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
         <v>31</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
       </c>
       <c r="E30" t="s">
         <v>32</v>
       </c>
       <c r="F30" t="s">
-        <v>33</v>
-      </c>
-      <c r="G30" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30">
+        <v>10</v>
+      </c>
+      <c r="G30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1763,25 +1673,22 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31">
         <v>30</v>
       </c>
-      <c r="E31" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" t="s">
-        <v>33</v>
-      </c>
-      <c r="G31" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1789,25 +1696,22 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32">
         <v>120</v>
       </c>
-      <c r="E32" t="s">
-        <v>35</v>
-      </c>
-      <c r="F32" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" t="s">
-        <v>14</v>
-      </c>
-      <c r="H32">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1815,25 +1719,22 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" t="s">
+        <v>32</v>
+      </c>
+      <c r="F33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33">
         <v>240</v>
       </c>
-      <c r="E33" t="s">
-        <v>36</v>
-      </c>
-      <c r="F33" t="s">
-        <v>33</v>
-      </c>
-      <c r="G33" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1841,25 +1742,22 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
       </c>
       <c r="E34" t="s">
         <v>32</v>
       </c>
       <c r="F34" t="s">
-        <v>33</v>
-      </c>
-      <c r="G34" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34">
+        <v>10</v>
+      </c>
+      <c r="G34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1867,25 +1765,22 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35">
         <v>30</v>
       </c>
-      <c r="E35" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" t="s">
-        <v>33</v>
-      </c>
-      <c r="G35" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1893,25 +1788,22 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36">
         <v>120</v>
       </c>
-      <c r="E36" t="s">
-        <v>35</v>
-      </c>
-      <c r="F36" t="s">
-        <v>33</v>
-      </c>
-      <c r="G36" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1919,25 +1811,22 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37">
         <v>240</v>
       </c>
-      <c r="E37" t="s">
-        <v>36</v>
-      </c>
-      <c r="F37" t="s">
-        <v>33</v>
-      </c>
-      <c r="G37" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1945,25 +1834,22 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F38" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38">
         <v>30</v>
       </c>
-      <c r="E38" t="s">
-        <v>37</v>
-      </c>
-      <c r="F38" t="s">
-        <v>33</v>
-      </c>
-      <c r="G38" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1971,25 +1857,22 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39">
+        <v>17</v>
+      </c>
+      <c r="D39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" t="s">
+        <v>32</v>
+      </c>
+      <c r="F39" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39">
         <v>120</v>
       </c>
-      <c r="E39" t="s">
-        <v>38</v>
-      </c>
-      <c r="F39" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" t="s">
-        <v>20</v>
-      </c>
-      <c r="H39">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1997,25 +1880,22 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40">
+        <v>17</v>
+      </c>
+      <c r="D40" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40">
         <v>240</v>
       </c>
-      <c r="E40" t="s">
-        <v>39</v>
-      </c>
-      <c r="F40" t="s">
-        <v>33</v>
-      </c>
-      <c r="G40" t="s">
-        <v>20</v>
-      </c>
-      <c r="H40">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2023,25 +1903,22 @@
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41">
+        <v>17</v>
+      </c>
+      <c r="D41" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F41" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41">
         <v>30</v>
       </c>
-      <c r="E41" t="s">
-        <v>37</v>
-      </c>
-      <c r="F41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G41" t="s">
-        <v>20</v>
-      </c>
-      <c r="H41">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2049,25 +1926,22 @@
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42">
+        <v>17</v>
+      </c>
+      <c r="D42" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" t="s">
+        <v>32</v>
+      </c>
+      <c r="F42" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42">
         <v>120</v>
       </c>
-      <c r="E42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F42" t="s">
-        <v>33</v>
-      </c>
-      <c r="G42" t="s">
-        <v>20</v>
-      </c>
-      <c r="H42">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2075,25 +1949,22 @@
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43">
+        <v>17</v>
+      </c>
+      <c r="D43" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F43" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43">
         <v>240</v>
       </c>
-      <c r="E43" t="s">
-        <v>39</v>
-      </c>
-      <c r="F43" t="s">
-        <v>33</v>
-      </c>
-      <c r="G43" t="s">
-        <v>20</v>
-      </c>
-      <c r="H43">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2101,25 +1972,22 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>39</v>
       </c>
       <c r="E44" t="s">
         <v>40</v>
       </c>
       <c r="F44" t="s">
-        <v>41</v>
-      </c>
-      <c r="G44" t="s">
-        <v>11</v>
-      </c>
-      <c r="H44">
+        <v>10</v>
+      </c>
+      <c r="G44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2127,25 +1995,22 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>12</v>
-      </c>
-      <c r="D45">
+        <v>11</v>
+      </c>
+      <c r="D45" t="s">
+        <v>41</v>
+      </c>
+      <c r="E45" t="s">
+        <v>40</v>
+      </c>
+      <c r="F45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45">
         <v>30</v>
       </c>
-      <c r="E45" t="s">
-        <v>42</v>
-      </c>
-      <c r="F45" t="s">
-        <v>41</v>
-      </c>
-      <c r="G45" t="s">
-        <v>14</v>
-      </c>
-      <c r="H45">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2153,25 +2018,22 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46">
+        <v>11</v>
+      </c>
+      <c r="D46" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" t="s">
+        <v>40</v>
+      </c>
+      <c r="F46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46">
         <v>120</v>
       </c>
-      <c r="E46" t="s">
-        <v>43</v>
-      </c>
-      <c r="F46" t="s">
-        <v>41</v>
-      </c>
-      <c r="G46" t="s">
-        <v>14</v>
-      </c>
-      <c r="H46">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2179,25 +2041,22 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
-      </c>
-      <c r="D47">
+        <v>11</v>
+      </c>
+      <c r="D47" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47">
         <v>240</v>
       </c>
-      <c r="E47" t="s">
-        <v>44</v>
-      </c>
-      <c r="F47" t="s">
-        <v>41</v>
-      </c>
-      <c r="G47" t="s">
-        <v>14</v>
-      </c>
-      <c r="H47">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2205,25 +2064,22 @@
         <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>39</v>
       </c>
       <c r="E48" t="s">
         <v>40</v>
       </c>
       <c r="F48" t="s">
-        <v>41</v>
-      </c>
-      <c r="G48" t="s">
-        <v>11</v>
-      </c>
-      <c r="H48">
+        <v>10</v>
+      </c>
+      <c r="G48">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2231,25 +2087,22 @@
         <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
-      </c>
-      <c r="D49">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s">
+        <v>41</v>
+      </c>
+      <c r="E49" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49">
         <v>30</v>
       </c>
-      <c r="E49" t="s">
-        <v>42</v>
-      </c>
-      <c r="F49" t="s">
-        <v>41</v>
-      </c>
-      <c r="G49" t="s">
-        <v>14</v>
-      </c>
-      <c r="H49">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2257,25 +2110,22 @@
         <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>12</v>
-      </c>
-      <c r="D50">
+        <v>11</v>
+      </c>
+      <c r="D50" t="s">
+        <v>42</v>
+      </c>
+      <c r="E50" t="s">
+        <v>40</v>
+      </c>
+      <c r="F50" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50">
         <v>120</v>
       </c>
-      <c r="E50" t="s">
-        <v>43</v>
-      </c>
-      <c r="F50" t="s">
-        <v>41</v>
-      </c>
-      <c r="G50" t="s">
-        <v>14</v>
-      </c>
-      <c r="H50">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2283,25 +2133,22 @@
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>12</v>
-      </c>
-      <c r="D51">
+        <v>11</v>
+      </c>
+      <c r="D51" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" t="s">
+        <v>40</v>
+      </c>
+      <c r="F51" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51">
         <v>240</v>
       </c>
-      <c r="E51" t="s">
-        <v>44</v>
-      </c>
-      <c r="F51" t="s">
-        <v>41</v>
-      </c>
-      <c r="G51" t="s">
-        <v>14</v>
-      </c>
-      <c r="H51">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2309,25 +2156,22 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>18</v>
-      </c>
-      <c r="D52">
+        <v>17</v>
+      </c>
+      <c r="D52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E52" t="s">
+        <v>40</v>
+      </c>
+      <c r="F52" t="s">
+        <v>19</v>
+      </c>
+      <c r="G52">
         <v>30</v>
       </c>
-      <c r="E52" t="s">
-        <v>45</v>
-      </c>
-      <c r="F52" t="s">
-        <v>41</v>
-      </c>
-      <c r="G52" t="s">
-        <v>20</v>
-      </c>
-      <c r="H52">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2335,25 +2179,22 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53">
+        <v>17</v>
+      </c>
+      <c r="D53" t="s">
+        <v>45</v>
+      </c>
+      <c r="E53" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53" t="s">
+        <v>19</v>
+      </c>
+      <c r="G53">
         <v>120</v>
       </c>
-      <c r="E53" t="s">
-        <v>46</v>
-      </c>
-      <c r="F53" t="s">
-        <v>41</v>
-      </c>
-      <c r="G53" t="s">
-        <v>20</v>
-      </c>
-      <c r="H53">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2361,25 +2202,22 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54">
+        <v>17</v>
+      </c>
+      <c r="D54" t="s">
+        <v>46</v>
+      </c>
+      <c r="E54" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54">
         <v>240</v>
       </c>
-      <c r="E54" t="s">
-        <v>47</v>
-      </c>
-      <c r="F54" t="s">
-        <v>41</v>
-      </c>
-      <c r="G54" t="s">
-        <v>20</v>
-      </c>
-      <c r="H54">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2387,25 +2225,22 @@
         <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>18</v>
-      </c>
-      <c r="D55">
+        <v>17</v>
+      </c>
+      <c r="D55" t="s">
+        <v>44</v>
+      </c>
+      <c r="E55" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" t="s">
+        <v>19</v>
+      </c>
+      <c r="G55">
         <v>30</v>
       </c>
-      <c r="E55" t="s">
-        <v>45</v>
-      </c>
-      <c r="F55" t="s">
-        <v>41</v>
-      </c>
-      <c r="G55" t="s">
-        <v>20</v>
-      </c>
-      <c r="H55">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2413,25 +2248,22 @@
         <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>18</v>
-      </c>
-      <c r="D56">
+        <v>17</v>
+      </c>
+      <c r="D56" t="s">
+        <v>45</v>
+      </c>
+      <c r="E56" t="s">
+        <v>40</v>
+      </c>
+      <c r="F56" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56">
         <v>120</v>
       </c>
-      <c r="E56" t="s">
-        <v>46</v>
-      </c>
-      <c r="F56" t="s">
-        <v>41</v>
-      </c>
-      <c r="G56" t="s">
-        <v>20</v>
-      </c>
-      <c r="H56">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2439,21 +2271,18 @@
         <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>18</v>
-      </c>
-      <c r="D57">
-        <v>240</v>
+        <v>17</v>
+      </c>
+      <c r="D57" t="s">
+        <v>46</v>
       </c>
       <c r="E57" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F57" t="s">
-        <v>41</v>
-      </c>
-      <c r="G57" t="s">
-        <v>20</v>
-      </c>
-      <c r="H57">
+        <v>19</v>
+      </c>
+      <c r="G57">
         <v>240</v>
       </c>
     </row>

</xml_diff>